<commit_message>
Reuploading Bug Report 0.2 and Locnew 33 video
Bug Locnew 33 explained further and report spellchecked
</commit_message>
<xml_diff>
--- a/Local News/Local News - Bug Report 0.2.xlsx
+++ b/Local News/Local News - Bug Report 0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22d1aaffb5e974dc/Desktop/Game Testing/Local News/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{AF51B4D8-35A7-4AEC-B391-605D2E5ACCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D800B28-ED9D-4445-AD29-0D6F41FAADD0}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{AF51B4D8-35A7-4AEC-B391-605D2E5ACCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{521037D7-8E5D-4380-BB76-16D826691B29}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="263">
   <si>
     <t>Defect Report</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>Priroty</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -456,9 +453,6 @@
     <t>Locnew 19</t>
   </si>
   <si>
-    <t>Player can move freely while talking to Oaklyin on day 1</t>
-  </si>
-  <si>
     <t>When Cliff and Clarence gets into their dialogue on day 1, the character artwork does not change when Cliff talks</t>
   </si>
   <si>
@@ -486,9 +480,6 @@
     <t>Player cannot move around while in dialogue</t>
   </si>
   <si>
-    <t>Player can move around while in dialogue with Oakliyn</t>
-  </si>
-  <si>
     <t>Locnew 20</t>
   </si>
   <si>
@@ -780,28 +771,49 @@
     <t>Finish the dialogue with Lyla after their father finishes repairing the car</t>
   </si>
   <si>
-    <t xml:space="preserve">Player can push Lyla and Cliff </t>
-  </si>
-  <si>
-    <t>Walking into Cliff causes him to run back facing the player while Lyla glithces away if player does the same</t>
-  </si>
-  <si>
-    <t>Finish the dialouge with Rose and Lyla</t>
-  </si>
-  <si>
     <t>Walk against Cliff</t>
   </si>
   <si>
-    <t>Walk againt Lyla</t>
-  </si>
-  <si>
     <t>NPCs do not get pushed away if player walks against them</t>
   </si>
   <si>
-    <t>Lyla and Cliff get pushed away if player walks against them</t>
-  </si>
-  <si>
     <t>15-07-2023 - 16-07-2023</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Finish the dialogue with Rose and Lyla</t>
+  </si>
+  <si>
+    <t>Walk against Lyla</t>
+  </si>
+  <si>
+    <t>Walk against Hoss</t>
+  </si>
+  <si>
+    <t>Walk against Clarence</t>
+  </si>
+  <si>
+    <t>Walk against Danny</t>
+  </si>
+  <si>
+    <t>Player can move freely while talking to Oaklyn on day 1</t>
+  </si>
+  <si>
+    <t>Player can move around while in dialogue with Oaklyn</t>
+  </si>
+  <si>
+    <t>Walk against Hot Doug</t>
+  </si>
+  <si>
+    <t>Player running against certain NPCs cause them to move away</t>
+  </si>
+  <si>
+    <t>Walking into certain NPCs causes them to move away on day 3</t>
+  </si>
+  <si>
+    <t>Certain NPCs get pushed away if player walks against them</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1264,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60820B4C-E762-4DB8-A5FB-C32065110B67}" name="Table2" displayName="Table2" ref="B11:H133" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="B11:H133" xr:uid="{60820B4C-E762-4DB8-A5FB-C32065110B67}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60820B4C-E762-4DB8-A5FB-C32065110B67}" name="Table2" displayName="Table2" ref="B11:H137" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="B11:H137" xr:uid="{60820B4C-E762-4DB8-A5FB-C32065110B67}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{7F2893E9-ADB1-4509-B0A9-4A944A97BD35}" name="BugID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{687076DE-3F2C-4B88-8671-ABD2542E7605}" name="Short Description" dataDxfId="5"/>
@@ -1261,7 +1273,7 @@
     <tableColumn id="4" xr3:uid="{074D4C42-8E50-47E3-944A-E73CA293C7B4}" name="Steps for Reproduction" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{D692C13A-45CB-460F-8EF0-628DBEC827ED}" name="Expected Result" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{6B66FD6C-B62D-4057-AAAB-B2E55F011589}" name="Actual Result" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{86C16205-DC5C-49AB-9C6A-8EDEF85DDC15}" name="Priroty" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{86C16205-DC5C-49AB-9C6A-8EDEF85DDC15}" name="Priority" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1530,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H133"/>
+  <dimension ref="B1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:H8"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1613,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -1649,30 +1661,30 @@
         <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>14</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="F12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1680,7 +1692,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1691,7 +1703,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -1708,25 +1720,25 @@
     </row>
     <row r="16" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="D16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="F16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1734,7 +1746,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1751,25 +1763,25 @@
     </row>
     <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="H19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1777,7 +1789,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1794,25 +1806,25 @@
     </row>
     <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="H22" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1820,7 +1832,7 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1831,7 +1843,7 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1842,7 +1854,7 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1859,25 +1871,25 @@
     </row>
     <row r="27" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="H27" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -1885,7 +1897,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1902,25 +1914,25 @@
     </row>
     <row r="30" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="F30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="H30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1928,7 +1940,7 @@
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1939,7 +1951,7 @@
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1956,25 +1968,25 @@
     </row>
     <row r="34" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="H34" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1982,7 +1994,7 @@
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1999,25 +2011,25 @@
     </row>
     <row r="37" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="E37" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F37" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="H37" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -2025,7 +2037,7 @@
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2036,7 +2048,7 @@
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2047,7 +2059,7 @@
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2064,25 +2076,25 @@
     </row>
     <row r="42" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="F42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G42" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="H42" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -2090,7 +2102,7 @@
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2101,7 +2113,7 @@
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2118,25 +2130,25 @@
     </row>
     <row r="46" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="F46" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
@@ -2144,7 +2156,7 @@
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -2161,25 +2173,25 @@
     </row>
     <row r="49" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="F49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G49" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G49" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="H49" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2187,7 +2199,7 @@
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -2204,25 +2216,25 @@
     </row>
     <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F52" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G52" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="H52" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
@@ -2230,7 +2242,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -2247,25 +2259,25 @@
     </row>
     <row r="55" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="D55" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="F55" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
@@ -2273,7 +2285,7 @@
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -2284,7 +2296,7 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -2295,7 +2307,7 @@
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -2306,7 +2318,7 @@
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -2317,7 +2329,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -2334,25 +2346,25 @@
     </row>
     <row r="62" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="E62" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="F62" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2360,7 +2372,7 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2371,7 +2383,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2388,25 +2400,25 @@
     </row>
     <row r="66" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="D66" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="E66" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="F66" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="G66" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G66" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="H66" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
@@ -2420,25 +2432,25 @@
     </row>
     <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="D68" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="E68" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E68" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="F68" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
@@ -2446,7 +2458,7 @@
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -2463,25 +2475,25 @@
     </row>
     <row r="71" spans="2:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D71" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="F71" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G71" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G71" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="H71" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
@@ -2489,7 +2501,7 @@
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -2500,7 +2512,7 @@
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -2511,7 +2523,7 @@
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -2522,7 +2534,7 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -2533,7 +2545,7 @@
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
@@ -2550,25 +2562,25 @@
     </row>
     <row r="78" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E78" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F78" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F78" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="G78" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2576,7 +2588,7 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -2593,25 +2605,25 @@
     </row>
     <row r="81" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>143</v>
+        <v>257</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E81" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F81" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F81" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="G81" s="4" t="s">
-        <v>153</v>
+        <v>258</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
@@ -2619,7 +2631,7 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -2636,25 +2648,25 @@
     </row>
     <row r="84" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="E84" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F84" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D84" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="G84" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
@@ -2668,25 +2680,25 @@
     </row>
     <row r="86" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B86" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E86" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E86" s="4" t="s">
+      <c r="F86" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F86" s="4" t="s">
-        <v>165</v>
-      </c>
       <c r="G86" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
@@ -2694,7 +2706,7 @@
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
@@ -2705,7 +2717,7 @@
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
@@ -2716,7 +2728,7 @@
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
@@ -2727,7 +2739,7 @@
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
@@ -2738,7 +2750,7 @@
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
@@ -2755,25 +2767,25 @@
     </row>
     <row r="93" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>170</v>
-      </c>
       <c r="F93" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
@@ -2781,7 +2793,7 @@
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -2792,7 +2804,7 @@
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
@@ -2803,7 +2815,7 @@
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
@@ -2814,7 +2826,7 @@
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
@@ -2825,7 +2837,7 @@
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
@@ -2836,7 +2848,7 @@
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
@@ -2853,25 +2865,25 @@
     </row>
     <row r="101" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="G101" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
@@ -2885,25 +2897,25 @@
     </row>
     <row r="103" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
@@ -2917,25 +2929,25 @@
     </row>
     <row r="105" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F105" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="G105" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="H105" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
@@ -2943,7 +2955,7 @@
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -2960,25 +2972,25 @@
     </row>
     <row r="108" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E108" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="F108" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="G108" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
@@ -2986,7 +2998,7 @@
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -3003,25 +3015,25 @@
     </row>
     <row r="111" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="D111" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G111" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="H111" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.25">
@@ -3029,7 +3041,7 @@
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
@@ -3040,7 +3052,7 @@
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -3057,25 +3069,25 @@
     </row>
     <row r="115" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E115" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E115" s="3" t="s">
+      <c r="F115" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="F115" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="G115" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.25">
@@ -3083,7 +3095,7 @@
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
@@ -3094,7 +3106,7 @@
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
@@ -3105,7 +3117,7 @@
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
@@ -3122,25 +3134,25 @@
     </row>
     <row r="120" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E120" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D120" s="3" t="s">
+      <c r="F120" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E120" s="3" t="s">
+      <c r="G120" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F120" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="H120" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
@@ -3148,7 +3160,7 @@
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -3165,25 +3177,25 @@
     </row>
     <row r="123" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C123" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E123" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="E123" s="3" t="s">
+      <c r="F123" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="F123" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="G123" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.25">
@@ -3191,7 +3203,7 @@
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
@@ -3202,7 +3214,7 @@
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -3228,25 +3240,25 @@
     </row>
     <row r="128" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D128" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F128" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E128" s="3" t="s">
+      <c r="G128" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="F128" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>248</v>
-      </c>
       <c r="H128" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -3254,7 +3266,7 @@
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
@@ -3269,27 +3281,27 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
     </row>
-    <row r="131" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F131" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C131" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="E131" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>256</v>
-      </c>
       <c r="G131" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
@@ -3297,7 +3309,7 @@
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
       <c r="E132" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
@@ -3308,11 +3320,55 @@
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
       <c r="E133" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+      <c r="H134" s="3"/>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
+      <c r="H135" s="3"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
+      <c r="H136" s="3"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>